<commit_message>
updates to other test data to include proper header
</commit_message>
<xml_diff>
--- a/test/data/sample_data.xlsx
+++ b/test/data/sample_data.xlsx
@@ -13,13 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
-    <t>rel angle</t>
+    <t>releaseAngle</t>
   </si>
   <si>
-    <t>length short arm</t>
+    <t>lengthArmShort</t>
   </si>
   <si>
-    <t>mass of wt</t>
+    <t>massWeight</t>
   </si>
 </sst>
 </file>
@@ -60,7 +60,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -83,13 +83,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -99,7 +161,25 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1152,16 +1232,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.5391" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.9062" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.8516" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1174,182 +1255,216 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>10</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>0.25</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>5</v>
       </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>20</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>0.5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>10</v>
       </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="3">
+      <c r="A4" s="5">
         <v>30</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>0.75</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>15</v>
       </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <v>40</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>20</v>
       </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="3">
+      <c r="A6" s="5">
         <v>50</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>1.25</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>25</v>
       </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="3">
+      <c r="A7" s="5">
         <v>60</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>1.5</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>30</v>
       </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="3">
+      <c r="A8" s="5">
         <v>70</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>1.75</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>35</v>
       </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <v>80</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>2</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>40</v>
       </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="3">
+      <c r="A10" s="5">
         <v>90</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>2.25</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>45</v>
       </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="3">
+      <c r="A11" s="5">
         <v>100</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>2.5</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>50</v>
       </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="3">
+      <c r="A12" s="5">
         <v>110</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>2.75</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
         <v>55</v>
       </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="3">
+      <c r="A13" s="5">
         <v>120</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>3</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
         <v>60</v>
       </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="3">
+      <c r="A14" s="5">
         <v>130</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="5">
         <v>3.25</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
         <v>65</v>
       </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="3">
+      <c r="A15" s="5">
         <v>140</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>3.5</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
         <v>70</v>
       </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="3">
+      <c r="A16" s="5">
         <v>150</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="5">
         <v>3.75</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="5">
         <v>75</v>
       </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="3">
+      <c r="A17" s="5">
         <v>160</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="5">
         <v>4</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="5">
         <v>80</v>
       </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>